<commit_message>
Fixed broken link in fields documentation.
</commit_message>
<xml_diff>
--- a/static/fields/drugenforcement_reference.xlsx
+++ b/static/fields/drugenforcement_reference.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28028"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="15820" tabRatio="500"/>
+    <workbookView xWindow="36380" yWindow="0" windowWidth="25360" windowHeight="15820" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="drug_enforcement_report" sheetId="1" r:id="rId1"/>
@@ -251,28 +251,20 @@
     <t>Section</t>
   </si>
   <si>
+    <t>See the OpenFDA fields section on the API Reference page https://open.fda.gov/apis/openfda-fields/) for list of openFDA fields.</t>
+  </si>
+  <si>
     <t>Different datasets use different drug identifiers—brand name, generic name, NDA, NDC, etc. It can be difficult to find the same drug in different datasets. And some identifiers, like pharmacologic class, are useful search filters but not available in all datasets.
 OpenFDA features harmonization of drug identifiers to make it easier to search enforcement report records by more identifiers, like product type (OTC versus prescription). Drug products that appear in enforcement reports are harmonized on NDC or UPC, if available. The linked data is listed as an openfda annotation in the patient.drug section of a result.
-Roughly half of enforcement reports have an openfda section. Because the harmonization process requires an exact match, some drug products cannot be harmonized in this fashion—for instance, if there is no NDC or UPC in the original enforcement report, there will be no openfda section.</t>
-  </si>
-  <si>
-    <t>See the OpenFDA fields section on the API Reference page (https://open.fda.gov/api/reference/) for list of openFDA fields.</t>
+Only a portion of enforcement reports have an openfda section. Because the harmonization process requires an exact match, some drug products cannot be harmonized in this fashion—for instance, if there is no NDC or UPC in the original enforcement report, there will be no openfda section.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -301,16 +293,35 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -318,69 +329,90 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="41">
@@ -758,16 +790,16 @@
   </sheetPr>
   <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="20" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="16.6640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.1640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.83203125" style="3"/>
-    <col min="4" max="4" width="118.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.83203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="107.5" style="3" customWidth="1"/>
     <col min="5" max="16384" width="10.83203125" style="3"/>
   </cols>
   <sheetData>
@@ -785,273 +817,274 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="255">
-      <c r="A2" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="4" t="s">
+    <row r="2" spans="1:4" ht="360">
+      <c r="A2" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" s="5" t="s">
+      <c r="C2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="6" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="360">
-      <c r="A3" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="4" t="s">
+    <row r="3" spans="1:4" ht="409">
+      <c r="A3" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D3" s="5" t="s">
+      <c r="C3" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="6" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="330">
-      <c r="A4" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="4" t="s">
+    <row r="4" spans="1:4" ht="409">
+      <c r="A4" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D4" s="5" t="s">
+      <c r="C4" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="6" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="45">
-      <c r="A5" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="4" t="s">
+    <row r="5" spans="1:4" ht="80">
+      <c r="A5" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D5" s="5" t="s">
+      <c r="C5" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" s="6" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:4">
-      <c r="A6" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="4" t="s">
+      <c r="A6" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D6" s="5" t="s">
+      <c r="C6" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D6" s="6" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="30">
-      <c r="A7" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B7" s="4" t="s">
+    <row r="7" spans="1:4" ht="40">
+      <c r="A7" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D7" s="5" t="s">
+      <c r="C7" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D7" s="6" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
-      <c r="A8" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B8" s="4" t="s">
+    <row r="8" spans="1:4" ht="40">
+      <c r="A8" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D8" s="5" t="s">
+      <c r="C8" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D8" s="6" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:4">
-      <c r="A9" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B9" s="4" t="s">
+      <c r="A9" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D9" s="5" t="s">
+      <c r="C9" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D9" s="6" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="300">
-      <c r="A10" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B10" s="4" t="s">
+    <row r="10" spans="1:4" ht="409">
+      <c r="A10" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D10" s="5" t="s">
+      <c r="C10" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D10" s="6" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:4">
-      <c r="A11" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B11" s="4" t="s">
+      <c r="A11" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C11" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D11" s="5" t="s">
+      <c r="C11" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D11" s="6" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="12" spans="1:4">
-      <c r="A12" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B12" s="4" t="s">
+      <c r="A12" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C12" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D12" s="3" t="s">
+      <c r="C12" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D12" s="4" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="255">
-      <c r="A13" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B13" s="4" t="s">
+    <row r="13" spans="1:4" ht="360">
+      <c r="A13" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B13" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C13" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D13" s="5" t="s">
+      <c r="C13" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D13" s="6" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="255">
-      <c r="A14" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B14" s="4" t="s">
+    <row r="14" spans="1:4" ht="340">
+      <c r="A14" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B14" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C14" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D14" s="5" t="s">
+      <c r="C14" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D14" s="6" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="15" spans="1:4">
-      <c r="A15" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B15" s="4" t="s">
+      <c r="A15" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B15" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C15" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D15" s="3" t="s">
+      <c r="C15" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D15" s="4" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="210">
-      <c r="A16" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B16" s="4" t="s">
+    <row r="16" spans="1:4" ht="280">
+      <c r="A16" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B16" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C16" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D16" s="5" t="s">
+      <c r="C16" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D16" s="6" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="240">
-      <c r="A17" s="3" t="s">
+    <row r="17" spans="1:4" ht="320">
+      <c r="A17" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B17" s="4" t="s">
+      <c r="B17" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C17" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D17" s="5" t="s">
+      <c r="C17" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D17" s="6" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="240">
-      <c r="A18" s="3" t="s">
+    <row r="18" spans="1:4" ht="320">
+      <c r="A18" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B18" s="4" t="s">
+      <c r="B18" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C18" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D18" s="5" t="s">
+      <c r="C18" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D18" s="6" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="240">
-      <c r="A19" s="3" t="s">
+    <row r="19" spans="1:4" ht="320">
+      <c r="A19" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B19" s="4" t="s">
+      <c r="B19" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C19" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D19" s="5" t="s">
+      <c r="C19" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D19" s="6" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="150">
-      <c r="A20" s="3" t="s">
+    <row r="20" spans="1:4" ht="260">
+      <c r="A20" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="B20" s="6" t="s">
+      <c r="B20" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="C20" s="4"/>
+      <c r="D20" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="D20" s="5" t="s">
-        <v>44</v>
-      </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="4" type="noConversion"/>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup scale="21" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup scale="51" fitToHeight="4" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="100"/>

</xml_diff>

<commit_message>
Fixed typo in drug enforcement reference documents.
</commit_message>
<xml_diff>
--- a/static/fields/drugenforcement_reference.xlsx
+++ b/static/fields/drugenforcement_reference.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28028"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10709"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jackfinch/WebstormProjects/open.fda.gov/static/fields/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32D5D7C8-FC30-414A-A88D-915AE683C3F5}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="36380" yWindow="0" windowWidth="25360" windowHeight="15820" tabRatio="500"/>
+    <workbookView xWindow="3440" yWindow="460" windowWidth="25360" windowHeight="15820" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="drug_enforcement_report" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="140000"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -19,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="44">
   <si>
     <t>Field Name</t>
   </si>
@@ -33,9 +39,6 @@
     <t>string</t>
   </si>
   <si>
-    <t>Enfocement report</t>
-  </si>
-  <si>
     <t>recalling_firm</t>
   </si>
   <si>
@@ -93,50 +96,6 @@
     <t>country</t>
   </si>
   <si>
-    <t>The firm that initiates a recall or, in the case of an FDA requested recall or FDA mandated recall, the firm that has primary responsibility for the manufacture and (or) marketing of the product to be recalled.
-This is an .exact field. It has been indexed both as its exact string content, and also tokenized.
-search=recalling_firm:"FOO+BAR"
-Searches for records where either FOO or BAR appear anywhere in this field.
-search=recalling_firm.exact:"FOO+BAR"
-Searches for records where exactly and only FOO BAR appears in this field.
-count=recalling_firm
-Counts the tokenized values of this field. Instances of FOO and BAR are counted separately.
-count=recalling_firm.exact
-Counts the exact values of this field. FOO BAR, BAR FOO, FOO, and BAR would all be counted separately, along with other combinations that contain these terms.</t>
-  </si>
-  <si>
-    <t>Numerical designation (I, II, or III) that is assigned by FDA to a particular product recall that indicates the relative degree of health hazard.
-This is an .exact field. It has been indexed both as its exact string content, and also tokenized.
-search=classification:"FOO+BAR"
-Searches for records where either FOO or BAR appear anywhere in this field.
-search=classification.exact:"FOO+BAR"
-Searches for records where exactly and only FOO BAR appears in this field.
-count=classification
-Counts the tokenized values of this field. Instances of FOO and BAR are counted separately.
-count=classification.exact
-Counts the exact values of this field. FOO BAR, BAR FOO, FOO, and BAR would all be counted separately, along with other combinations that contain these terms.
-Value is one of the following
-Class I = Dangerous or defective products that predictably could cause serious health problems or death. Examples include: food found to contain botulinum toxin, food with undeclared allergens, a label mix-up on a lifesaving drug, or a defective artificial heart valve.
-Class II = Products that might cause a temporary health problem, or pose only a slight threat of a serious nature. Example: a drug that is under-strength but that is not used to treat life-threatening situations.
-Class III = Products that are unlikely to cause any adverse health reaction, but that violate FDA labeling or manufacturing laws. Examples include: a minor container defect and lack of English labeling in a retail food.</t>
-  </si>
-  <si>
-    <t>This is an .exact field. It has been indexed both as its exact string content, and also tokenized.
-search=status:"FOO+BAR"
-Searches for records where either FOO or BAR appear anywhere in this field.
-search=status.exact:"FOO+BAR"
-Searches for records where exactly and only FOO BAR appears in this field.
-count=status
-Counts the tokenized values of this field. Instances of FOO and BAR are counted separately.
-count=status.exact
-Counts the exact values of this field. FOO BAR, BAR FOO, FOO, and BAR would all be counted separately, along with other combinations that contain these terms.
-Value is one of the following
-On-Going = A recall which is currently in progress.
-Completed = The recall action reaches the point at which the firm has actually retrieved and impounded all outstanding product that could reasonably be expected to be recovered, or has completed all product corrections.
-Terminated = FDA has determined that all reasonable efforts have been made to remove or correct the violative product in accordance with the recall strategy, and proper disposition has been made according to the degree of hazard.
-Pending = Actions that have been determined to be recalls, but that remain in the process of being classified.</t>
-  </si>
-  <si>
     <t>General area of initial distribution such as, “Distributors in 6 states: NY, VA, TX, GA, FL and MA; the Virgin Islands; Canada and Japan”. The term “nationwide” is defined to mean the fifty states or a significant portion. Note that subsequent distribution by the consignees to other parties may not be included.</t>
   </si>
   <si>
@@ -152,97 +111,13 @@
     <t>The amount of defective product subject to recall.</t>
   </si>
   <si>
-    <t>Describes who initiated the recall. Recalls are almost always voluntary, meaning initiated by a firm. A recall is deemed voluntary when the firm voluntarily removes or corrects marketed products or the FDA requests the marketed products be removed or corrected. A recall is mandated when the firm was ordered by the FDA to remove or correct the marketed products, under section 518(e) of the FD&amp;C Act, National Childhood Vaccine Injury Act of 1986, 21 CFR 1271.440, Infant Formula Act of 1980 and its 1986 amendments, or the Food Safety Modernization Act (FSMA).
-This is an .exact field. It has been indexed both as its exact string content, and also tokenized.
-search=voluntary_mandated:"FOO+BAR"
-Searches for records where either FOO or BAR appear anywhere in this field.
-search=voluntary_mandated.exact:"FOO+BAR"
-Searches for records where exactly and only FOO BAR appears in this field.
-count=voluntary_mandated
-Counts the tokenized values of this field. Instances of FOO and BAR are counted separately.
-count=voluntary_mandated.exact
-Counts the exact values of this field. FOO BAR, BAR FOO, FOO, and BAR would all be counted separately, along with other combinations that contain these terms.</t>
-  </si>
-  <si>
     <t>Date that the FDA issued the enforcement report for the product recall.</t>
   </si>
   <si>
     <t>Date that the firm first began notifying the public or their consignees of the recall.</t>
   </si>
   <si>
-    <t>The method(s) by which the firm initially notified the public or their consignees of a recall. A consignee is a person or firm named in a bill of lading to whom or to whose order the product has or will be delivered.
-This is an .exact field. It has been indexed both as its exact string content, and also tokenized.
-search=initial_firm_notification:"FOO+BAR"
-Searches for records where either FOO or BAR appear anywhere in this field.
-search=initial_firm_notification.exact:"FOO+BAR"
-Searches for records where exactly and only FOO BAR appears in this field.
-count=initial_firm_notification
-Counts the tokenized values of this field. Instances of FOO and BAR are counted separately.
-count=initial_firm_notification.exact
-Counts the exact values of this field. FOO BAR, BAR FOO, FOO, and BAR would all be counted separately, along with other combinations that contain these terms.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A numerical designation assigned by FDA to a specific recall event used for tracking purposes.
-This is an .exact field. It has been indexed both as its exact string content, and also tokenized.
-search=recall_number:"FOO+BAR"
-Searches for records where either FOO or BAR appear anywhere in this field.
-search=recall_number.exact:"FOO+BAR"
-Searches for records where exactly and only FOO BAR appears in this field.
-count=recall_number
-Counts the tokenized values of this field. Instances of FOO and BAR are counted separately.
-count=recall_number.exact
-Counts the exact values of this field. FOO BAR, BAR FOO, FOO, and BAR would all be counted separately, along with other combinations that contain these terms.
-</t>
-  </si>
-  <si>
     <t>A numerical designation assigned by FDA to a specific recall event used for tracking purposes.</t>
-  </si>
-  <si>
-    <t>This is an .exact field. It has been indexed both as its exact string content, and also tokenized.
-search=product_type:"FOO+BAR"
-Searches for records where either FOO or BAR appear anywhere in this field.
-search=product_type.exact:"FOO+BAR"
-Searches for records where exactly and only FOO BAR appears in this field.
-count=product_type
-Counts the tokenized values of this field. Instances of FOO and BAR are counted separately.
-count=product_type.exact
-Counts the exact values of this field. FOO BAR, BAR FOO, FOO, and BAR would all be counted separately, along with other combinations that contain these terms.</t>
-  </si>
-  <si>
-    <t>The city in which the recalling firm is located.
-This is an .exact field. It has been indexed both as its exact string content, and also tokenized.
-search=city:"FOO+BAR"
-Searches for records where either FOO or BAR appear anywhere in this field.
-search=city.exact:"FOO+BAR"
-Searches for records where exactly and only FOO BAR appears in this field.
-count=city
-Counts the tokenized values of this field. Instances of FOO and BAR are counted separately.
-count=city.exact
-Counts the exact values of this field. FOO BAR, BAR FOO, FOO, and BAR would all be counted separately, along with other combinations that contain these terms.</t>
-  </si>
-  <si>
-    <t>The U.S. state in which the recalling firm is located.
-This is an .exact field. It has been indexed both as its exact string content, and also tokenized.
-search=state:"FOO+BAR"
-Searches for records where either FOO or BAR appear anywhere in this field.
-search=state.exact:"FOO+BAR"
-Searches for records where exactly and only FOO BAR appears in this field.
-count=state
-Counts the tokenized values of this field. Instances of FOO and BAR are counted separately.
-count=state.exact
-Counts the exact values of this field. FOO BAR, BAR FOO, FOO, and BAR would all be counted separately, along with other combinations that contain these terms.</t>
-  </si>
-  <si>
-    <t>The country in which the recalling firm is located.
-This is an .exact field. It has been indexed both as its exact string content, and also tokenized.
-search=country:"FOO+BAR"
-Searches for records where either FOO or BAR appear anywhere in this field.
-search=country.exact:"FOO+BAR"
-Searches for records where exactly and only FOO BAR appears in this field.
-count=country
-Counts the tokenized values of this field. Instances of FOO and BAR are counted separately.
-count=country.exact
-Counts the exact values of this field. FOO BAR, BAR FOO, FOO, and BAR would all be counted separately, along with other combinations that contain these terms.</t>
   </si>
   <si>
     <t>openFDA</t>
@@ -257,12 +132,39 @@
     <t>Different datasets use different drug identifiers—brand name, generic name, NDA, NDC, etc. It can be difficult to find the same drug in different datasets. And some identifiers, like pharmacologic class, are useful search filters but not available in all datasets.
 OpenFDA features harmonization of drug identifiers to make it easier to search enforcement report records by more identifiers, like product type (OTC versus prescription). Drug products that appear in enforcement reports are harmonized on NDC or UPC, if available. The linked data is listed as an openfda annotation in the patient.drug section of a result.
 Only a portion of enforcement reports have an openfda section. Because the harmonization process requires an exact match, some drug products cannot be harmonized in this fashion—for instance, if there is no NDC or UPC in the original enforcement report, there will be no openfda section.</t>
+  </si>
+  <si>
+    <t>Enforcement report</t>
+  </si>
+  <si>
+    <t>The firm that initiates a recall or, in the case of an FDA requested recall or FDA mandated recall, the firm that has primary responsibility for the manufacture and (or) marketing of the product to be recalled.</t>
+  </si>
+  <si>
+    <t>Numerical designation (I, II, or III) that is assigned by FDA to a particular product recall that indicates the relative degree of health hazard.</t>
+  </si>
+  <si>
+    <t>Describes who initiated the recall. Recalls are almost always voluntary, meaning initiated by a firm. A recall is deemed voluntary when the firm voluntarily removes or corrects marketed products or the FDA requests the marketed products be removed or corrected. A recall is mandated when the firm was ordered by the FDA to remove or correct the marketed products, under section 518(e) of the FD&amp;C Act, National Childhood Vaccine Injury Act of 1986, 21 CFR 1271.440, Infant Formula Act of 1980 and its 1986 amendments, or the Food Safety Modernization Act (FSMA).</t>
+  </si>
+  <si>
+    <t>The method(s) by which the firm initially notified the public or their consignees of a recall. A consignee is a person or firm named in a bill of lading to whom or to whose order the product has or will be delivered.</t>
+  </si>
+  <si>
+    <t>The type of product being recalled. For drug queries, this will always be `Drugs`.</t>
+  </si>
+  <si>
+    <t>The city in which the recalling firm is located.</t>
+  </si>
+  <si>
+    <t>The U.S. state in which the recalling firm is located.</t>
+  </si>
+  <si>
+    <t>The country in which the recalling firm is located.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -460,6 +362,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -784,28 +694,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="20" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="22.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="27.33203125" style="8" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7.83203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="107.5" style="3" customWidth="1"/>
+    <col min="4" max="4" width="79.1640625" style="3" customWidth="1"/>
     <col min="5" max="16384" width="10.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -817,274 +727,273 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="360">
+    <row r="2" spans="1:4" ht="63" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="C2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="42" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B3" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" s="6" t="s">
+      <c r="C3" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="6"/>
+    </row>
+    <row r="5" spans="1:4" ht="105" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D6" s="6" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="409">
-      <c r="A3" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D3" s="6" t="s">
+    <row r="7" spans="1:4" ht="63" x14ac:dyDescent="0.2">
+      <c r="A7" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D7" s="6" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="409">
-      <c r="A4" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D4" s="6" t="s">
+    <row r="8" spans="1:4" ht="42" x14ac:dyDescent="0.2">
+      <c r="A8" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D8" s="6" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="80">
-      <c r="A5" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D5" s="6" t="s">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D9" s="6" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
-      <c r="A6" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D6" s="6" t="s">
+    <row r="10" spans="1:4" ht="168" x14ac:dyDescent="0.2">
+      <c r="A10" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D11" s="6" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="40">
-      <c r="A7" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D7" s="6" t="s">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D12" s="4" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="40">
-      <c r="A8" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D8" s="6" t="s">
+    <row r="13" spans="1:4" ht="63" x14ac:dyDescent="0.2">
+      <c r="A13" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="42" x14ac:dyDescent="0.2">
+      <c r="A14" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D14" s="6" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
-      <c r="A9" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D9" s="6" t="s">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="42" x14ac:dyDescent="0.2">
+      <c r="A16" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="315" x14ac:dyDescent="0.2">
+      <c r="A20" s="4" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" ht="409">
-      <c r="A10" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="A11" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D11" s="6" t="s">
+      <c r="B20" s="7" t="s">
         <v>33</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
-      <c r="A12" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="360">
-      <c r="A13" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D13" s="6" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="340">
-      <c r="A14" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D14" s="6" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4">
-      <c r="A15" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="280">
-      <c r="A16" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D16" s="6" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="320">
-      <c r="A17" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B17" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D17" s="6" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="320">
-      <c r="A18" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B18" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D18" s="6" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="320">
-      <c r="A19" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B19" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D19" s="6" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="260">
-      <c r="A20" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="B20" s="7" t="s">
-        <v>44</v>
       </c>
       <c r="C20" s="4"/>
       <c r="D20" s="6" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
+  <printOptions gridLines="1"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup scale="51" fitToHeight="4" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup fitToWidth="0" fitToHeight="4" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="100"/>

</xml_diff>